<commit_message>
My New Final MVN Cucumber Project
</commit_message>
<xml_diff>
--- a/MAVEN/src/test/resources/AppTest.xlsx
+++ b/MAVEN/src/test/resources/AppTest.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>url</t>
   </si>
@@ -714,6 +714,12 @@
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">

</xml_diff>